<commit_message>
HLAT: Updates on multi-run handling (basic submit).
</commit_message>
<xml_diff>
--- a/examples/manifest_example.xlsx
+++ b/examples/manifest_example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucsdhs-my.sharepoint.com/personal/aphodges_health_ucsd_edu/Documents/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\drew\builds\cast\hla_typing\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FC67175-A9B8-43FA-BBA1-6F851BCDF624}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28DB17E-0D05-423F-92CE-5C6B54325FF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5640" xr2:uid="{6C50DA76-A255-4560-9001-14352591B095}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>ID</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>sample3.cram</t>
+  </si>
+  <si>
+    <t>Target Cram</t>
+  </si>
+  <si>
+    <t>/local/sample1.cram</t>
+  </si>
+  <si>
+    <t>/local/sample2.cram</t>
+  </si>
+  <si>
+    <t>/local/sample3.cram</t>
   </si>
 </sst>
 </file>
@@ -75,8 +87,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,43 +404,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{706BBE4F-3CDF-46FF-9C58-F33387E2661E}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -437,6 +463,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010051D8D7DAE46052428E9D6A7CD98694EF" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0700d6bf0c269e04816ef787034d60df">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3d49e5ce-37d7-4ef0-89c8-0e8b57491c0f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b040c1bf283b269cb185972e8995658c" ns3:_="">
     <xsd:import namespace="3d49e5ce-37d7-4ef0-89c8-0e8b57491c0f"/>
@@ -594,22 +635,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95BD2206-AF26-4DCB-922C-5FE83AC30F23}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3d49e5ce-37d7-4ef0-89c8-0e8b57491c0f"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B35D33A2-E7B2-4A9C-AB61-E05928E11B7B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EFFD4F3-D3DB-44CF-9F39-402C690C7C5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -625,28 +675,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B35D33A2-E7B2-4A9C-AB61-E05928E11B7B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95BD2206-AF26-4DCB-922C-5FE83AC30F23}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3d49e5ce-37d7-4ef0-89c8-0e8b57491c0f"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>